<commit_message>
Modernisation de la collection Revenus dans le formulaire d'édition de la cotation
</commit_message>
<xml_diff>
--- a/Template du SOA.xlsx
+++ b/Template du SOA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JSBrokers_1_0_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAB3CE5-0A56-406B-9D94-3ECC91AA1B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3131A620-C4E0-44EA-83C2-1507C0A3E7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13470" yWindow="-5565" windowWidth="13500" windowHeight="10980" xr2:uid="{F6D134A9-AAB0-457E-AD9F-16F2EB0CA2A4}"/>
+    <workbookView xWindow="-20025" yWindow="-5790" windowWidth="16095" windowHeight="12000" xr2:uid="{F6D134A9-AAB0-457E-AD9F-16F2EB0CA2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Prime nette</t>
   </si>
@@ -65,9 +65,6 @@
     <t>2e Tranche</t>
   </si>
   <si>
-    <t>Comm. Ordinaire HT</t>
-  </si>
-  <si>
     <t>Taxe Assureur (ex: Tva)</t>
   </si>
   <si>
@@ -102,6 +99,18 @@
   </si>
   <si>
     <t>Solde</t>
+  </si>
+  <si>
+    <t>Montant encaissé</t>
+  </si>
+  <si>
+    <t>Date d'encaissement</t>
+  </si>
+  <si>
+    <t>Montant Payé</t>
+  </si>
+  <si>
+    <t>Comm. Ordinaire HT (10%)</t>
   </si>
 </sst>
 </file>
@@ -156,7 +165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -176,6 +185,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB345BF2-437D-4F24-BA9F-25AAF95E8FC9}">
-  <dimension ref="D1:K26"/>
+  <dimension ref="D1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +553,7 @@
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -632,177 +642,296 @@
       </c>
     </row>
     <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5">
+        <v>146</v>
+      </c>
+      <c r="F9" s="5">
+        <v>73</v>
+      </c>
+      <c r="G9" s="5">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="F10" s="9">
+        <v>46023</v>
+      </c>
+      <c r="G10" s="9">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <f>E8-E9</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" ref="F11:G11" si="2">F8-F9</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1">
+        <f>E16-E17</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F15" s="1">
+        <f>F16-F17</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G15" s="1">
+        <f>G16-G17</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1">
         <f>10%*E4</f>
         <v>10</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" ref="F13:F16" si="2">E13*$F$2</f>
+      <c r="F16" s="1">
+        <f t="shared" ref="F16:F19" si="3">E16*$F$2</f>
         <v>5</v>
       </c>
-      <c r="G13" s="1">
-        <f t="shared" ref="G13:G16" si="3">E13*$G$2</f>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G19" si="4">E16*$G$2</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1">
-        <f>2%*E13</f>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <f>2%*E16</f>
         <v>0.2</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F17" s="1">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1">
-        <f>16%*E13</f>
+      <c r="G17" s="1">
+        <f t="shared" si="4"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1">
+        <f>16%*E16</f>
         <v>1.6</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F18" s="1">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="4" t="s">
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="5">
-        <f>E15+E13</f>
+      <c r="E19" s="5">
+        <f>E18+E16</f>
         <v>11.6</v>
       </c>
-      <c r="F16" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8</v>
-      </c>
-      <c r="G16" s="5">
+      <c r="F19" s="5">
         <f t="shared" si="3"/>
         <v>5.8</v>
       </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="1">
-        <f>E13-E14</f>
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="F17" s="1">
-        <f>F13-F14</f>
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="G17" s="1">
-        <f>G13-G14</f>
-        <v>4.9000000000000004</v>
+      <c r="G19" s="5">
+        <f t="shared" si="4"/>
+        <v>5.8</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="F20">
+        <v>5.8</v>
+      </c>
+      <c r="G20">
+        <v>5.8</v>
+      </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="F21" s="9">
+        <v>46023</v>
+      </c>
+      <c r="G21" s="9">
+        <v>46054</v>
       </c>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1">
+        <f>E19-E20</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" ref="F22:G22" si="5">F19-F20</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1">
+        <f>E15</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F28" s="1">
+        <f>F15</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G28" s="1">
+        <f>G15</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="7">
         <v>0.35</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="1">
-        <f>E22*E17</f>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1">
+        <f>E29*E28</f>
         <v>3.43</v>
       </c>
-      <c r="F23" s="1">
-        <f>E23*$F$2</f>
+      <c r="F30" s="1">
+        <f>E30*$F$2</f>
         <v>1.7150000000000001</v>
       </c>
-      <c r="G23">
-        <f t="shared" ref="G23" si="4">E23*$G$2</f>
+      <c r="G30" s="1">
+        <f>E30*$G$2</f>
         <v>1.7150000000000001</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="1">
+        <f>F31+G31</f>
+        <v>3.43</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1.7150000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F24">
-        <v>1.7150000000000001</v>
-      </c>
-      <c r="G24">
-        <v>1.7150000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
+      <c r="F32" s="9">
+        <v>46023</v>
+      </c>
+      <c r="G32" s="9">
+        <v>46054</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
-        <v>21</v>
+      <c r="E33" s="1">
+        <f>E30-E31</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <f>F30-F31</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <f>G30-G31</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D14:G14"/>
     <mergeCell ref="D3:G3"/>
-    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="D26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>